<commit_message>
supdate authors and Source
</commit_message>
<xml_diff>
--- a/other/reginfo.xlsx
+++ b/other/reginfo.xlsx
@@ -624,9 +624,6 @@
     <t>Shaomin</t>
   </si>
   <si>
-    <t>CHEN</t>
-  </si>
-  <si>
     <t>Tsinghua University</t>
   </si>
   <si>
@@ -2401,6 +2398,9 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>Lawrence Berkeley National Laboratory and University of California, Berkeley</t>
   </si>
 </sst>
 </file>
@@ -2781,8 +2781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -3723,16 +3723,16 @@
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="F28" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="G28" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>204</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>8</v>
@@ -3752,20 +3752,20 @@
         <v>5</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F29" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>208</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>34</v>
@@ -3785,22 +3785,22 @@
         <v>5</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D30" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>211</v>
       </c>
       <c r="F30" s="7">
         <v>5056033708</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>8</v>
@@ -3820,13 +3820,13 @@
         <v>25</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>35</v>
@@ -3835,7 +3835,7 @@
         <v>7737101898</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>8</v>
@@ -3859,16 +3859,16 @@
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F32" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="G32" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>2</v>
@@ -3888,22 +3888,22 @@
         <v>25</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F33" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>222</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>8</v>
@@ -3929,16 +3929,16 @@
         <v>6</v>
       </c>
       <c r="D34" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="F34" s="7">
         <v>6507032473</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>8</v>
@@ -3965,7 +3965,7 @@
         <v>48</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>49</v>
@@ -3974,7 +3974,7 @@
         <v>8128554590</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>2</v>
@@ -3992,11 +3992,11 @@
     <row r="36" spans="1:12">
       <c r="A36" s="6"/>
       <c r="B36" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>50</v>
@@ -4005,7 +4005,7 @@
         <v>8148635943</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H36" s="6" t="s">
         <v>8</v>
@@ -4026,20 +4026,20 @@
     <row r="37" spans="1:12">
       <c r="A37" s="6"/>
       <c r="B37" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F37" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="G37" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>234</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>24</v>
@@ -4059,20 +4059,20 @@
         <v>5</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F38" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="G38" s="6" t="s">
         <v>237</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>238</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>34</v>
@@ -4092,20 +4092,20 @@
         <v>25</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="F39" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="G39" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>243</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>24</v>
@@ -4131,7 +4131,7 @@
         <v>52</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>37</v>
@@ -4140,7 +4140,7 @@
         <v>8655765229</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>24</v>
@@ -4164,16 +4164,16 @@
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>37</v>
       </c>
       <c r="F41" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="G41" s="6" t="s">
         <v>247</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>248</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>8</v>
@@ -4193,11 +4193,11 @@
         <v>5</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>54</v>
@@ -4206,7 +4206,7 @@
         <v>5104991929</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H42" s="6" t="s">
         <v>2</v>
@@ -4224,20 +4224,20 @@
     <row r="43" spans="1:12">
       <c r="A43" s="6"/>
       <c r="B43" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>254</v>
       </c>
       <c r="F43" s="7">
         <v>5178845715</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H43" s="6" t="s">
         <v>24</v>
@@ -4255,22 +4255,22 @@
     <row r="44" spans="1:12">
       <c r="A44" s="6"/>
       <c r="B44" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="D44" s="6" t="s">
         <v>257</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>258</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F44" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="G44" s="6" t="s">
         <v>259</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>260</v>
       </c>
       <c r="H44" s="6" t="s">
         <v>34</v>
@@ -4290,11 +4290,11 @@
         <v>5</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>55</v>
@@ -4303,7 +4303,7 @@
         <v>6302527549</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H45" s="6" t="s">
         <v>8</v>
@@ -4326,13 +4326,13 @@
         <v>5</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>56</v>
@@ -4341,7 +4341,7 @@
         <v>2158956860</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H46" s="6" t="s">
         <v>8</v>
@@ -4363,16 +4363,16 @@
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F47" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="G47" s="6" t="s">
         <v>268</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>269</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>34</v>
@@ -4390,20 +4390,20 @@
     <row r="48" spans="1:12">
       <c r="A48" s="6"/>
       <c r="B48" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F48" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="G48" s="6" t="s">
         <v>272</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>273</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>24</v>
@@ -4429,16 +4429,16 @@
         <v>15</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>54</v>
       </c>
       <c r="F49" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="G49" s="6" t="s">
         <v>275</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>276</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>8</v>
@@ -4462,16 +4462,16 @@
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>277</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>278</v>
       </c>
       <c r="F50" s="7">
         <v>4126249244</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>24</v>
@@ -4491,20 +4491,20 @@
         <v>25</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>60</v>
       </c>
       <c r="F51" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="G51" s="6" t="s">
         <v>282</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>283</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>8</v>
@@ -4530,7 +4530,7 @@
         <v>48</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>62</v>
@@ -4539,7 +4539,7 @@
         <v>6086956320</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>24</v>
@@ -4559,20 +4559,20 @@
         <v>5</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>63</v>
       </c>
       <c r="F53" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="G53" s="6" t="s">
         <v>288</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>24</v>
@@ -4592,20 +4592,20 @@
         <v>25</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F54" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="G54" s="6" t="s">
         <v>292</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>293</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>24</v>
@@ -4623,20 +4623,20 @@
     <row r="55" spans="1:13">
       <c r="A55" s="6"/>
       <c r="B55" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F55" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="G55" s="6" t="s">
         <v>296</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>297</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>8</v>
@@ -4659,20 +4659,20 @@
         <v>5</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F56" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="G56" s="6" t="s">
         <v>300</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>301</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>24</v>
@@ -4701,7 +4701,7 @@
         <v>65</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>54</v>
@@ -4710,7 +4710,7 @@
         <v>5104864398</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>8</v>
@@ -4734,16 +4734,16 @@
         <v>65</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>67</v>
       </c>
       <c r="F58" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="G58" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>306</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>24</v>
@@ -4763,20 +4763,20 @@
         <v>25</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C59" s="6"/>
       <c r="D59" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="F59" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="F59" s="7" t="s">
+      <c r="G59" s="6" t="s">
         <v>310</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>311</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>24</v>
@@ -4802,16 +4802,16 @@
         <v>68</v>
       </c>
       <c r="D60" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="F60" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="F60" s="7" t="s">
+      <c r="G60" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>315</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>8</v>
@@ -4831,11 +4831,11 @@
         <v>5</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>37</v>
@@ -4844,7 +4844,7 @@
         <v>8655746124</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>8</v>
@@ -4864,22 +4864,22 @@
         <v>5</v>
       </c>
       <c r="B62" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="C62" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="D62" s="6" t="s">
         <v>320</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>321</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F62" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="G62" s="6" t="s">
         <v>322</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>323</v>
       </c>
       <c r="H62" s="6" t="s">
         <v>8</v>
@@ -4902,20 +4902,20 @@
         <v>19</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C63" s="6"/>
       <c r="D63" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="E63" s="6" t="s">
         <v>325</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>326</v>
       </c>
       <c r="F63" s="7">
         <v>9846142632</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H63" s="6" t="s">
         <v>2</v>
@@ -4935,20 +4935,20 @@
         <v>19</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C64" s="6"/>
       <c r="D64" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="E64" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="E64" s="6" t="s">
+      <c r="F64" s="7" t="s">
         <v>330</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="G64" s="6" t="s">
         <v>331</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>332</v>
       </c>
       <c r="H64" s="6" t="s">
         <v>8</v>
@@ -4968,13 +4968,13 @@
         <v>5</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>40</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>69</v>
@@ -4983,7 +4983,7 @@
         <v>5073018908</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H65" s="6" t="s">
         <v>2</v>
@@ -5003,11 +5003,11 @@
         <v>25</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>70</v>
@@ -5016,7 +5016,7 @@
         <v>6316327971</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H66" s="6" t="s">
         <v>24</v>
@@ -5037,22 +5037,22 @@
     <row r="67" spans="1:13">
       <c r="A67" s="6"/>
       <c r="B67" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>55</v>
       </c>
       <c r="F67" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="G67" s="6" t="s">
         <v>341</v>
-      </c>
-      <c r="G67" s="6" t="s">
-        <v>342</v>
       </c>
       <c r="H67" s="6" t="s">
         <v>8</v>
@@ -5072,20 +5072,20 @@
         <v>5</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F68" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="G68" s="6" t="s">
         <v>345</v>
-      </c>
-      <c r="G68" s="6" t="s">
-        <v>346</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>34</v>
@@ -5106,11 +5106,11 @@
     <row r="69" spans="1:13">
       <c r="A69" s="6"/>
       <c r="B69" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>1</v>
@@ -5119,7 +5119,7 @@
         <v>2039016607</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>2</v>
@@ -5142,10 +5142,10 @@
         <v>71</v>
       </c>
       <c r="C70" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="D70" s="6" t="s">
         <v>350</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>351</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>37</v>
@@ -5154,7 +5154,7 @@
         <v>6502488775</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H70" s="6" t="s">
         <v>8</v>
@@ -5171,10 +5171,10 @@
     </row>
     <row r="71" spans="1:13">
       <c r="B71" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="D71" t="s">
         <v>353</v>
-      </c>
-      <c r="D71" t="s">
-        <v>354</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>63</v>
@@ -5201,7 +5201,7 @@
         <v>6313442088</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H72" s="6" t="s">
         <v>34</v>
@@ -5219,7 +5219,7 @@
     <row r="73" spans="1:13">
       <c r="A73" s="6"/>
       <c r="B73" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="6" t="s">
@@ -5232,7 +5232,7 @@
         <v>6318917245</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H73" s="6" t="s">
         <v>2</v>
@@ -5250,20 +5250,20 @@
     <row r="74" spans="1:13">
       <c r="A74" s="6"/>
       <c r="B74" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>62</v>
       </c>
       <c r="F74" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="G74" s="6" t="s">
         <v>360</v>
-      </c>
-      <c r="G74" s="6" t="s">
-        <v>361</v>
       </c>
       <c r="H74" s="6" t="s">
         <v>8</v>
@@ -5281,20 +5281,20 @@
     <row r="75" spans="1:13">
       <c r="A75" s="6"/>
       <c r="B75" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C75" s="6"/>
       <c r="D75" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F75" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="G75" s="6" t="s">
         <v>364</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>365</v>
       </c>
       <c r="H75" s="6" t="s">
         <v>8</v>
@@ -5314,20 +5314,20 @@
         <v>5</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C76" s="6"/>
       <c r="D76" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F76" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="G76" s="6" t="s">
         <v>368</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>369</v>
       </c>
       <c r="H76" s="6" t="s">
         <v>34</v>
@@ -5347,11 +5347,11 @@
         <v>5</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C77" s="6"/>
       <c r="D77" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>30</v>
@@ -5360,7 +5360,7 @@
         <v>6308404545</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H77" s="6" t="s">
         <v>8</v>
@@ -5380,13 +5380,13 @@
         <v>25</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>1</v>
@@ -5395,7 +5395,7 @@
         <v>4752012702</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H78" s="6" t="s">
         <v>8</v>
@@ -5425,16 +5425,16 @@
       </c>
       <c r="C79" s="6"/>
       <c r="D79" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="E79" s="6" t="s">
+      <c r="F79" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="F79" s="7" t="s">
+      <c r="G79" s="6" t="s">
         <v>378</v>
-      </c>
-      <c r="G79" s="6" t="s">
-        <v>379</v>
       </c>
       <c r="H79" s="6" t="s">
         <v>2</v>
@@ -5454,11 +5454,11 @@
         <v>5</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C80" s="6"/>
       <c r="D80" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>33</v>
@@ -5467,7 +5467,7 @@
         <v>2802</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H80" s="6" t="s">
         <v>34</v>
@@ -5491,16 +5491,16 @@
       </c>
       <c r="C81" s="6"/>
       <c r="D81" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>35</v>
       </c>
       <c r="F81" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="G81" s="6" t="s">
         <v>384</v>
-      </c>
-      <c r="G81" s="6" t="s">
-        <v>385</v>
       </c>
       <c r="H81" s="6" t="s">
         <v>8</v>
@@ -5520,20 +5520,20 @@
         <v>5</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C82" s="6"/>
       <c r="D82" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="E82" s="6" t="s">
         <v>387</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>388</v>
       </c>
       <c r="F82" s="7">
         <v>2076797159</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>8</v>
@@ -5557,16 +5557,16 @@
       </c>
       <c r="C83" s="6"/>
       <c r="D83" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="E83" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="E83" s="6" t="s">
+      <c r="F83" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="F83" s="7" t="s">
+      <c r="G83" s="6" t="s">
         <v>392</v>
-      </c>
-      <c r="G83" s="6" t="s">
-        <v>393</v>
       </c>
       <c r="H83" s="6" t="s">
         <v>8</v>
@@ -5586,11 +5586,11 @@
         <v>25</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>11</v>
@@ -5599,7 +5599,7 @@
         <v>5402318727</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H84" s="6" t="s">
         <v>8</v>
@@ -5626,7 +5626,7 @@
         <v>40</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>33</v>
@@ -5635,7 +5635,7 @@
         <v>6313445518</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H85" s="6" t="s">
         <v>34</v>
@@ -5653,22 +5653,22 @@
     <row r="86" spans="1:13">
       <c r="A86" s="6"/>
       <c r="B86" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>76</v>
       </c>
       <c r="F86" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="G86" s="6" t="s">
         <v>401</v>
-      </c>
-      <c r="G86" s="6" t="s">
-        <v>402</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>24</v>
@@ -5688,20 +5688,20 @@
         <v>5</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C87" s="6"/>
       <c r="D87" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E87" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F87" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="G87" s="6" t="s">
         <v>405</v>
-      </c>
-      <c r="G87" s="6" t="s">
-        <v>406</v>
       </c>
       <c r="H87" s="6" t="s">
         <v>34</v>
@@ -5721,20 +5721,20 @@
         <v>5</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C88" s="6"/>
       <c r="D88" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="E88" s="6" t="s">
         <v>408</v>
       </c>
-      <c r="E88" s="6" t="s">
+      <c r="F88" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="F88" s="7" t="s">
+      <c r="G88" s="6" t="s">
         <v>410</v>
-      </c>
-      <c r="G88" s="6" t="s">
-        <v>411</v>
       </c>
       <c r="H88" s="6" t="s">
         <v>8</v>
@@ -5758,16 +5758,16 @@
       </c>
       <c r="C89" s="6"/>
       <c r="D89" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E89" s="6" t="s">
         <v>49</v>
       </c>
       <c r="F89" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="G89" s="6" t="s">
         <v>413</v>
-      </c>
-      <c r="G89" s="6" t="s">
-        <v>414</v>
       </c>
       <c r="H89" s="6" t="s">
         <v>8</v>
@@ -5785,11 +5785,11 @@
     <row r="90" spans="1:13">
       <c r="A90" s="6"/>
       <c r="B90" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C90" s="6"/>
       <c r="D90" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>30</v>
@@ -5798,7 +5798,7 @@
         <v>6308408196</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H90" s="6" t="s">
         <v>24</v>
@@ -5819,10 +5819,10 @@
         <v>36</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>33</v>
@@ -5831,7 +5831,7 @@
         <v>6313445323</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H91" s="6" t="s">
         <v>34</v>
@@ -5859,16 +5859,16 @@
       </c>
       <c r="C92" s="6"/>
       <c r="D92" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F92" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="G92" s="6" t="s">
         <v>421</v>
-      </c>
-      <c r="G92" s="6" t="s">
-        <v>422</v>
       </c>
       <c r="H92" s="6" t="s">
         <v>34</v>
@@ -5894,7 +5894,7 @@
         <v>52</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>33</v>
@@ -5903,7 +5903,7 @@
         <v>6313445879</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H93" s="6" t="s">
         <v>34</v>
@@ -5927,16 +5927,16 @@
         <v>6</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E94" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F94" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="G94" s="6" t="s">
         <v>426</v>
-      </c>
-      <c r="G94" s="6" t="s">
-        <v>427</v>
       </c>
       <c r="H94" s="6" t="s">
         <v>8</v>
@@ -5962,13 +5962,13 @@
         <v>25</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>79</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E95" s="6" t="s">
         <v>80</v>
@@ -5977,7 +5977,7 @@
         <v>5106429619</v>
       </c>
       <c r="G95" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H95" s="6" t="s">
         <v>8</v>
@@ -6006,16 +6006,16 @@
         <v>10</v>
       </c>
       <c r="D96" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="E96" s="6" t="s">
         <v>431</v>
       </c>
-      <c r="E96" s="6" t="s">
+      <c r="F96" s="7" t="s">
         <v>432</v>
       </c>
-      <c r="F96" s="7" t="s">
+      <c r="G96" s="6" t="s">
         <v>433</v>
-      </c>
-      <c r="G96" s="6" t="s">
-        <v>434</v>
       </c>
       <c r="H96" s="6" t="s">
         <v>8</v>
@@ -6035,22 +6035,22 @@
         <v>25</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>40</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E97" s="6" t="s">
         <v>56</v>
       </c>
       <c r="F97" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="G97" s="6" t="s">
         <v>437</v>
-      </c>
-      <c r="G97" s="6" t="s">
-        <v>438</v>
       </c>
       <c r="H97" s="6" t="s">
         <v>8</v>
@@ -6076,7 +6076,7 @@
         <v>52</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E98" s="6" t="s">
         <v>1</v>
@@ -6085,7 +6085,7 @@
         <v>2402710217</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H98" s="6" t="s">
         <v>2</v>
@@ -6106,20 +6106,20 @@
     <row r="99" spans="1:13">
       <c r="A99" s="6"/>
       <c r="B99" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C99" s="6"/>
       <c r="D99" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E99" s="6" t="s">
         <v>42</v>
       </c>
       <c r="F99" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="G99" s="6" t="s">
         <v>443</v>
-      </c>
-      <c r="G99" s="6" t="s">
-        <v>444</v>
       </c>
       <c r="H99" s="6" t="s">
         <v>8</v>
@@ -6139,20 +6139,20 @@
         <v>25</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C100" s="6"/>
       <c r="D100" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E100" s="6" t="s">
         <v>81</v>
       </c>
       <c r="F100" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="G100" s="6" t="s">
         <v>447</v>
-      </c>
-      <c r="G100" s="6" t="s">
-        <v>448</v>
       </c>
       <c r="H100" s="6" t="s">
         <v>8</v>
@@ -6172,22 +6172,22 @@
         <v>25</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>79</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E101" s="6" t="s">
         <v>82</v>
       </c>
       <c r="F101" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="G101" s="6" t="s">
         <v>451</v>
-      </c>
-      <c r="G101" s="6" t="s">
-        <v>452</v>
       </c>
       <c r="H101" s="6" t="s">
         <v>8</v>
@@ -6207,11 +6207,11 @@
         <v>5</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C102" s="6"/>
       <c r="D102" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E102" s="6" t="s">
         <v>83</v>
@@ -6220,7 +6220,7 @@
         <v>6307652589</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H102" s="6" t="s">
         <v>2</v>
@@ -6246,16 +6246,16 @@
         <v>10</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E103" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F103" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="G103" s="6" t="s">
         <v>457</v>
-      </c>
-      <c r="G103" s="6" t="s">
-        <v>458</v>
       </c>
       <c r="H103" s="6" t="s">
         <v>24</v>
@@ -6283,16 +6283,16 @@
       </c>
       <c r="C104" s="6"/>
       <c r="D104" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F104" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="G104" s="6" t="s">
         <v>460</v>
-      </c>
-      <c r="G104" s="6" t="s">
-        <v>461</v>
       </c>
       <c r="H104" s="6" t="s">
         <v>34</v>
@@ -6315,20 +6315,20 @@
         <v>5</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C105" s="6"/>
       <c r="D105" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E105" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F105" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="G105" s="6" t="s">
         <v>464</v>
-      </c>
-      <c r="G105" s="6" t="s">
-        <v>465</v>
       </c>
       <c r="H105" s="6" t="s">
         <v>34</v>
@@ -6351,13 +6351,13 @@
         <v>25</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E106" s="6" t="s">
         <v>30</v>
@@ -6366,7 +6366,7 @@
         <v>6083548279</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H106" s="6" t="s">
         <v>8</v>
@@ -6389,20 +6389,20 @@
         <v>19</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C107" s="6"/>
       <c r="D107" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="E107" s="6" t="s">
         <v>470</v>
-      </c>
-      <c r="E107" s="6" t="s">
-        <v>471</v>
       </c>
       <c r="F107" s="7">
         <v>7185015309</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H107" s="6" t="s">
         <v>8</v>
@@ -6420,20 +6420,20 @@
     <row r="108" spans="1:13">
       <c r="A108" s="6"/>
       <c r="B108" s="6" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C108" s="6"/>
       <c r="D108" s="6" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F108" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="G108" s="6" t="s">
         <v>475</v>
-      </c>
-      <c r="G108" s="6" t="s">
-        <v>476</v>
       </c>
       <c r="H108" s="6" t="s">
         <v>2</v>
@@ -6451,20 +6451,20 @@
     <row r="109" spans="1:13" ht="30">
       <c r="A109" s="6"/>
       <c r="B109" s="6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C109" s="6"/>
       <c r="D109" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="E109" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="E109" s="6" t="s">
+      <c r="F109" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="F109" s="7" t="s">
+      <c r="G109" s="6" t="s">
         <v>480</v>
-      </c>
-      <c r="G109" s="6" t="s">
-        <v>481</v>
       </c>
       <c r="H109" s="6" t="s">
         <v>8</v>
@@ -6490,16 +6490,16 @@
         <v>68</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E110" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F110" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="G110" s="6" t="s">
         <v>483</v>
-      </c>
-      <c r="G110" s="6" t="s">
-        <v>484</v>
       </c>
       <c r="H110" s="6" t="s">
         <v>8</v>
@@ -6520,20 +6520,20 @@
     <row r="111" spans="1:13">
       <c r="A111" s="6"/>
       <c r="B111" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C111" s="6"/>
       <c r="D111" s="6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E111" s="6" t="s">
         <v>80</v>
       </c>
       <c r="F111" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="G111" s="6" t="s">
         <v>487</v>
-      </c>
-      <c r="G111" s="6" t="s">
-        <v>488</v>
       </c>
       <c r="H111" s="6" t="s">
         <v>8</v>
@@ -6550,10 +6550,10 @@
     </row>
     <row r="112" spans="1:13">
       <c r="B112" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="D112" s="6" t="s">
         <v>489</v>
-      </c>
-      <c r="D112" s="6" t="s">
-        <v>490</v>
       </c>
       <c r="E112" s="6" t="s">
         <v>30</v>
@@ -6579,7 +6579,7 @@
         <v>52</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E113" s="6" t="s">
         <v>33</v>
@@ -6588,7 +6588,7 @@
         <v>6313443151</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H113" s="6" t="s">
         <v>34</v>
@@ -6608,11 +6608,11 @@
         <v>25</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C114" s="6"/>
       <c r="D114" s="6" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E114" s="6" t="s">
         <v>82</v>
@@ -6621,7 +6621,7 @@
         <v>8082061742</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H114" s="6" t="s">
         <v>24</v>
@@ -6644,22 +6644,22 @@
         <v>25</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D115" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="E115" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="E115" s="6" t="s">
+      <c r="F115" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="F115" s="7" t="s">
+      <c r="G115" s="6" t="s">
         <v>499</v>
-      </c>
-      <c r="G115" s="6" t="s">
-        <v>500</v>
       </c>
       <c r="H115" s="6" t="s">
         <v>8</v>
@@ -6685,7 +6685,7 @@
         <v>15</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E116" s="6" t="s">
         <v>69</v>
@@ -6694,7 +6694,7 @@
         <v>2193169749</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H116" s="6" t="s">
         <v>2</v>
@@ -6718,16 +6718,16 @@
       </c>
       <c r="C117" s="6"/>
       <c r="D117" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E117" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F117" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="G117" s="6" t="s">
         <v>504</v>
-      </c>
-      <c r="G117" s="6" t="s">
-        <v>505</v>
       </c>
       <c r="H117" s="6" t="s">
         <v>8</v>
@@ -6747,20 +6747,20 @@
         <v>5</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C118" s="6"/>
       <c r="D118" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="E118" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="E118" s="6" t="s">
-        <v>508</v>
       </c>
       <c r="F118" s="7">
         <v>447737461854</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H118" s="6" t="s">
         <v>8</v>
@@ -6778,11 +6778,11 @@
     <row r="119" spans="1:12">
       <c r="A119" s="6"/>
       <c r="B119" s="6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C119" s="6"/>
       <c r="D119" s="6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E119" s="6" t="s">
         <v>30</v>
@@ -6791,7 +6791,7 @@
         <v>6308402193</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H119" s="6" t="s">
         <v>8</v>
@@ -6815,16 +6815,16 @@
       </c>
       <c r="C120" s="6"/>
       <c r="D120" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="E120" s="6" t="s">
         <v>513</v>
-      </c>
-      <c r="E120" s="6" t="s">
-        <v>514</v>
       </c>
       <c r="F120" s="7">
         <v>7734013299</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H120" s="6" t="s">
         <v>2</v>
@@ -6848,16 +6848,16 @@
       </c>
       <c r="C121" s="6"/>
       <c r="D121" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="E121" s="6" t="s">
         <v>516</v>
-      </c>
-      <c r="E121" s="6" t="s">
-        <v>517</v>
       </c>
       <c r="F121" s="7">
         <v>6263902073</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="H121" s="6" t="s">
         <v>8</v>
@@ -6881,16 +6881,16 @@
       </c>
       <c r="C122" s="6"/>
       <c r="D122" s="6" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E122" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F122" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="G122" s="6" t="s">
         <v>520</v>
-      </c>
-      <c r="G122" s="6" t="s">
-        <v>521</v>
       </c>
       <c r="H122" s="6" t="s">
         <v>24</v>
@@ -6908,11 +6908,11 @@
     <row r="123" spans="1:12">
       <c r="A123" s="6"/>
       <c r="B123" s="6" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C123" s="6"/>
       <c r="D123" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E123" s="6" t="s">
         <v>50</v>
@@ -6921,7 +6921,7 @@
         <v>8054532850</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H123" s="6" t="s">
         <v>8</v>
@@ -6941,20 +6941,20 @@
         <v>25</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C124" s="6"/>
       <c r="D124" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="E124" s="6" t="s">
         <v>526</v>
-      </c>
-      <c r="E124" s="6" t="s">
-        <v>527</v>
       </c>
       <c r="F124" s="7">
         <v>8058933440</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H124" s="6" t="s">
         <v>24</v>
@@ -6983,7 +6983,7 @@
         <v>6</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E125" s="6" t="s">
         <v>33</v>
@@ -6992,7 +6992,7 @@
         <v>6099178510</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H125" s="6" t="s">
         <v>34</v>
@@ -7012,22 +7012,22 @@
         <v>5</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C126" s="6" t="s">
         <v>79</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E126" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F126" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="G126" s="6" t="s">
         <v>533</v>
-      </c>
-      <c r="G126" s="6" t="s">
-        <v>534</v>
       </c>
       <c r="H126" s="6" t="s">
         <v>8</v>
@@ -7048,20 +7048,20 @@
     <row r="127" spans="1:12">
       <c r="A127" s="6"/>
       <c r="B127" s="6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C127" s="6"/>
       <c r="D127" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="E127" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="E127" s="6" t="s">
+      <c r="F127" s="7" t="s">
         <v>537</v>
       </c>
-      <c r="F127" s="7" t="s">
+      <c r="G127" s="6" t="s">
         <v>538</v>
-      </c>
-      <c r="G127" s="6" t="s">
-        <v>539</v>
       </c>
       <c r="H127" s="6" t="s">
         <v>8</v>
@@ -7085,16 +7085,16 @@
       </c>
       <c r="C128" s="6"/>
       <c r="D128" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="E128" s="6" t="s">
         <v>540</v>
       </c>
-      <c r="E128" s="6" t="s">
+      <c r="F128" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="F128" s="7" t="s">
+      <c r="G128" s="6" t="s">
         <v>542</v>
-      </c>
-      <c r="G128" s="6" t="s">
-        <v>543</v>
       </c>
       <c r="H128" s="6" t="s">
         <v>8</v>
@@ -7114,11 +7114,11 @@
         <v>25</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C129" s="6"/>
       <c r="D129" s="6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E129" s="6" t="s">
         <v>56</v>
@@ -7127,7 +7127,7 @@
         <v>2158952729</v>
       </c>
       <c r="G129" s="6" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H129" s="6" t="s">
         <v>8</v>
@@ -7151,16 +7151,16 @@
       </c>
       <c r="C130" s="6"/>
       <c r="D130" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="E130" s="6" t="s">
         <v>547</v>
       </c>
-      <c r="E130" s="6" t="s">
+      <c r="F130" s="7" t="s">
         <v>548</v>
       </c>
-      <c r="F130" s="7" t="s">
+      <c r="G130" s="6" t="s">
         <v>549</v>
-      </c>
-      <c r="G130" s="6" t="s">
-        <v>550</v>
       </c>
       <c r="H130" s="6" t="s">
         <v>8</v>
@@ -7180,20 +7180,20 @@
         <v>25</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C131" s="6"/>
       <c r="D131" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="E131" s="6" t="s">
         <v>552</v>
-      </c>
-      <c r="E131" s="6" t="s">
-        <v>553</v>
       </c>
       <c r="F131" s="7">
         <v>41764870463</v>
       </c>
       <c r="G131" s="6" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="H131" s="6" t="s">
         <v>8</v>
@@ -7217,20 +7217,20 @@
     <row r="132" spans="1:13">
       <c r="A132" s="6"/>
       <c r="B132" s="6" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C132" s="6"/>
       <c r="D132" s="6" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E132" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F132" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="G132" s="6" t="s">
         <v>557</v>
-      </c>
-      <c r="G132" s="6" t="s">
-        <v>558</v>
       </c>
       <c r="H132" s="6" t="s">
         <v>2</v>
@@ -7250,20 +7250,20 @@
         <v>5</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C133" s="6"/>
       <c r="D133" s="6" t="s">
+        <v>559</v>
+      </c>
+      <c r="E133" s="6" t="s">
         <v>560</v>
-      </c>
-      <c r="E133" s="6" t="s">
-        <v>561</v>
       </c>
       <c r="F133" s="7">
         <v>5129659473</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H133" s="6" t="s">
         <v>2</v>
@@ -7289,16 +7289,16 @@
         <v>6</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E134" s="6" t="s">
         <v>41</v>
       </c>
       <c r="F134" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="G134" s="6" t="s">
         <v>564</v>
-      </c>
-      <c r="G134" s="6" t="s">
-        <v>565</v>
       </c>
       <c r="H134" s="6" t="s">
         <v>24</v>
@@ -7313,7 +7313,7 @@
         <v>42020.820729166699</v>
       </c>
     </row>
-    <row r="135" spans="1:13">
+    <row r="135" spans="1:13" ht="30">
       <c r="A135" s="6" t="s">
         <v>25</v>
       </c>
@@ -7324,16 +7324,16 @@
         <v>43</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>54</v>
+        <v>793</v>
       </c>
       <c r="F135" s="7">
         <v>5104958235</v>
       </c>
       <c r="G135" s="6" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H135" s="6" t="s">
         <v>8</v>
@@ -7354,11 +7354,11 @@
     <row r="136" spans="1:13">
       <c r="A136" s="6"/>
       <c r="B136" s="6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C136" s="6"/>
       <c r="D136" s="6" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E136" s="6" t="s">
         <v>30</v>
@@ -7367,7 +7367,7 @@
         <v>6308403622</v>
       </c>
       <c r="G136" s="6" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H136" s="6" t="s">
         <v>8</v>
@@ -7387,20 +7387,20 @@
         <v>5</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C137" s="6"/>
       <c r="D137" s="6" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E137" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F137" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="G137" s="6" t="s">
         <v>573</v>
-      </c>
-      <c r="G137" s="6" t="s">
-        <v>574</v>
       </c>
       <c r="H137" s="6" t="s">
         <v>34</v>
@@ -7418,20 +7418,20 @@
     <row r="138" spans="1:13">
       <c r="A138" s="6"/>
       <c r="B138" s="6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C138" s="6"/>
       <c r="D138" s="6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E138" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F138" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="G138" s="6" t="s">
         <v>577</v>
-      </c>
-      <c r="G138" s="6" t="s">
-        <v>578</v>
       </c>
       <c r="H138" s="6" t="s">
         <v>24</v>
@@ -7455,16 +7455,16 @@
       </c>
       <c r="C139" s="6"/>
       <c r="D139" s="6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E139" s="6" t="s">
         <v>70</v>
       </c>
       <c r="F139" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="G139" s="6" t="s">
         <v>580</v>
-      </c>
-      <c r="G139" s="6" t="s">
-        <v>581</v>
       </c>
       <c r="H139" s="6" t="s">
         <v>8</v>
@@ -7484,20 +7484,20 @@
         <v>25</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C140" s="6"/>
       <c r="D140" s="6" t="s">
+        <v>582</v>
+      </c>
+      <c r="E140" s="6" t="s">
         <v>583</v>
       </c>
-      <c r="E140" s="6" t="s">
+      <c r="F140" s="7" t="s">
         <v>584</v>
       </c>
-      <c r="F140" s="7" t="s">
+      <c r="G140" s="6" t="s">
         <v>585</v>
-      </c>
-      <c r="G140" s="6" t="s">
-        <v>586</v>
       </c>
       <c r="H140" s="6" t="s">
         <v>8</v>
@@ -7517,20 +7517,20 @@
         <v>19</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C141" s="6"/>
       <c r="D141" s="6" t="s">
+        <v>587</v>
+      </c>
+      <c r="E141" s="6" t="s">
         <v>588</v>
       </c>
-      <c r="E141" s="6" t="s">
+      <c r="F141" s="7" t="s">
         <v>589</v>
       </c>
-      <c r="F141" s="7" t="s">
+      <c r="G141" s="6" t="s">
         <v>590</v>
-      </c>
-      <c r="G141" s="6" t="s">
-        <v>591</v>
       </c>
       <c r="H141" s="6" t="s">
         <v>8</v>
@@ -7550,20 +7550,20 @@
         <v>5</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C142" s="6"/>
       <c r="D142" s="6" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E142" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F142" s="7" t="s">
+        <v>593</v>
+      </c>
+      <c r="G142" s="6" t="s">
         <v>594</v>
-      </c>
-      <c r="G142" s="6" t="s">
-        <v>595</v>
       </c>
       <c r="H142" s="6" t="s">
         <v>34</v>
@@ -7587,11 +7587,11 @@
     <row r="143" spans="1:13">
       <c r="A143" s="6"/>
       <c r="B143" s="6" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C143" s="6"/>
       <c r="D143" s="6" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E143" s="6" t="s">
         <v>30</v>
@@ -7600,7 +7600,7 @@
         <v>6308408044</v>
       </c>
       <c r="G143" s="6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="H143" s="6" t="s">
         <v>8</v>
@@ -7618,20 +7618,20 @@
     <row r="144" spans="1:13">
       <c r="A144" s="6"/>
       <c r="B144" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C144" s="6"/>
       <c r="D144" s="6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E144" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F144" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="G144" s="6" t="s">
         <v>601</v>
-      </c>
-      <c r="G144" s="6" t="s">
-        <v>602</v>
       </c>
       <c r="H144" s="6" t="s">
         <v>8</v>
@@ -7657,20 +7657,20 @@
         <v>5</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C145" s="6"/>
       <c r="D145" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="E145" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="E145" s="6" t="s">
+      <c r="F145" s="7" t="s">
         <v>605</v>
       </c>
-      <c r="F145" s="7" t="s">
+      <c r="G145" s="6" t="s">
         <v>606</v>
-      </c>
-      <c r="G145" s="6" t="s">
-        <v>607</v>
       </c>
       <c r="H145" s="6" t="s">
         <v>24</v>
@@ -7690,20 +7690,20 @@
         <v>25</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C146" s="6"/>
       <c r="D146" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="E146" s="6" t="s">
         <v>609</v>
-      </c>
-      <c r="E146" s="6" t="s">
-        <v>610</v>
       </c>
       <c r="F146" s="7">
         <v>4126564725</v>
       </c>
       <c r="G146" s="6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="H146" s="6" t="s">
         <v>8</v>
@@ -7727,16 +7727,16 @@
       </c>
       <c r="C147" s="6"/>
       <c r="D147" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="E147" s="6" t="s">
         <v>612</v>
       </c>
-      <c r="E147" s="6" t="s">
+      <c r="F147" s="7" t="s">
         <v>613</v>
       </c>
-      <c r="F147" s="7" t="s">
+      <c r="G147" s="6" t="s">
         <v>614</v>
-      </c>
-      <c r="G147" s="6" t="s">
-        <v>615</v>
       </c>
       <c r="H147" s="6" t="s">
         <v>8</v>
@@ -7756,22 +7756,22 @@
         <v>19</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C148" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D148" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="E148" s="6" t="s">
         <v>617</v>
-      </c>
-      <c r="E148" s="6" t="s">
-        <v>618</v>
       </c>
       <c r="F148" s="7">
         <v>9103153669</v>
       </c>
       <c r="G148" s="6" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="H148" s="6" t="s">
         <v>2</v>
@@ -7789,20 +7789,20 @@
     <row r="149" spans="1:13">
       <c r="A149" s="6"/>
       <c r="B149" s="6" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C149" s="6"/>
       <c r="D149" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="E149" s="6" t="s">
         <v>621</v>
-      </c>
-      <c r="E149" s="6" t="s">
-        <v>622</v>
       </c>
       <c r="F149" s="7">
         <v>5852758529</v>
       </c>
       <c r="G149" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H149" s="6" t="s">
         <v>2</v>
@@ -7820,20 +7820,20 @@
     <row r="150" spans="1:13">
       <c r="A150" s="6"/>
       <c r="B150" s="6" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C150" s="6"/>
       <c r="D150" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="E150" s="6" t="s">
         <v>625</v>
-      </c>
-      <c r="E150" s="6" t="s">
-        <v>626</v>
       </c>
       <c r="F150" s="7">
         <v>8652967581</v>
       </c>
       <c r="G150" s="6" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="H150" s="6" t="s">
         <v>2</v>
@@ -7853,13 +7853,13 @@
         <v>25</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C151" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E151" s="6" t="s">
         <v>31</v>
@@ -7868,7 +7868,7 @@
         <v>5152947881</v>
       </c>
       <c r="G151" s="6" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="H151" s="6" t="s">
         <v>8</v>
@@ -7890,16 +7890,16 @@
       </c>
       <c r="C152" s="6"/>
       <c r="D152" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E152" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F152" s="7" t="s">
+        <v>631</v>
+      </c>
+      <c r="G152" s="6" t="s">
         <v>632</v>
-      </c>
-      <c r="G152" s="6" t="s">
-        <v>633</v>
       </c>
       <c r="H152" s="6" t="s">
         <v>34</v>
@@ -7925,16 +7925,16 @@
         <v>43</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E153" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F153" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="G153" s="6" t="s">
         <v>635</v>
-      </c>
-      <c r="G153" s="6" t="s">
-        <v>636</v>
       </c>
       <c r="H153" s="6" t="s">
         <v>2</v>
@@ -7954,20 +7954,20 @@
         <v>19</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C154" s="6"/>
       <c r="D154" s="6" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E154" s="6" t="s">
         <v>60</v>
       </c>
       <c r="F154" s="7" t="s">
+        <v>638</v>
+      </c>
+      <c r="G154" s="6" t="s">
         <v>639</v>
-      </c>
-      <c r="G154" s="6" t="s">
-        <v>640</v>
       </c>
       <c r="H154" s="6" t="s">
         <v>2</v>
@@ -7987,20 +7987,20 @@
         <v>25</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C155" s="6"/>
       <c r="D155" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="E155" s="6" t="s">
         <v>642</v>
       </c>
-      <c r="E155" s="6" t="s">
+      <c r="F155" s="7" t="s">
         <v>643</v>
       </c>
-      <c r="F155" s="7" t="s">
+      <c r="G155" s="6" t="s">
         <v>644</v>
-      </c>
-      <c r="G155" s="6" t="s">
-        <v>645</v>
       </c>
       <c r="H155" s="6" t="s">
         <v>24</v>
@@ -8025,7 +8025,7 @@
       </c>
       <c r="C156" s="6"/>
       <c r="D156" s="6" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="E156" s="6" t="s">
         <v>70</v>
@@ -8034,7 +8034,7 @@
         <v>6313717222</v>
       </c>
       <c r="G156" s="6" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H156" s="6" t="s">
         <v>2</v>
@@ -8056,16 +8056,16 @@
       </c>
       <c r="C157" s="6"/>
       <c r="D157" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E157" s="6" t="s">
         <v>35</v>
       </c>
       <c r="F157" s="7" t="s">
+        <v>648</v>
+      </c>
+      <c r="G157" s="6" t="s">
         <v>649</v>
-      </c>
-      <c r="G157" s="6" t="s">
-        <v>650</v>
       </c>
       <c r="H157" s="6" t="s">
         <v>8</v>
@@ -8088,11 +8088,11 @@
         <v>25</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C158" s="6"/>
       <c r="D158" s="6" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E158" s="6" t="s">
         <v>26</v>
@@ -8101,7 +8101,7 @@
         <v>9196602962</v>
       </c>
       <c r="G158" s="6" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="H158" s="6" t="s">
         <v>24</v>
@@ -8131,16 +8131,16 @@
       </c>
       <c r="C159" s="6"/>
       <c r="D159" s="6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="E159" s="6" t="s">
         <v>67</v>
       </c>
       <c r="F159" s="7" t="s">
+        <v>654</v>
+      </c>
+      <c r="G159" s="6" t="s">
         <v>655</v>
-      </c>
-      <c r="G159" s="6" t="s">
-        <v>656</v>
       </c>
       <c r="H159" s="6" t="s">
         <v>8</v>
@@ -8158,11 +8158,11 @@
     <row r="160" spans="1:13">
       <c r="A160" s="6"/>
       <c r="B160" s="6" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C160" s="6"/>
       <c r="D160" s="6" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E160" s="6" t="s">
         <v>38</v>
@@ -8171,7 +8171,7 @@
         <v>9145912806</v>
       </c>
       <c r="G160" s="6" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H160" s="6" t="s">
         <v>8</v>
@@ -8201,7 +8201,7 @@
       </c>
       <c r="C161" s="6"/>
       <c r="D161" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E161" s="6" t="s">
         <v>70</v>
@@ -8210,7 +8210,7 @@
         <v>6316327986</v>
       </c>
       <c r="G161" s="6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="H161" s="6" t="s">
         <v>24</v>
@@ -8236,7 +8236,7 @@
         <v>87</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E162" s="6" t="s">
         <v>42</v>
@@ -8245,7 +8245,7 @@
         <v>9498247502</v>
       </c>
       <c r="G162" s="6" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H162" s="6" t="s">
         <v>8</v>
@@ -8266,20 +8266,20 @@
     <row r="163" spans="1:13">
       <c r="A163" s="6"/>
       <c r="B163" s="6" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C163" s="6"/>
       <c r="D163" s="6" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E163" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F163" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="G163" s="6" t="s">
         <v>666</v>
-      </c>
-      <c r="G163" s="6" t="s">
-        <v>667</v>
       </c>
       <c r="H163" s="6" t="s">
         <v>8</v>
@@ -8299,20 +8299,20 @@
         <v>5</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C164" s="6"/>
       <c r="D164" s="6" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E164" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F164" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="G164" s="6" t="s">
         <v>670</v>
-      </c>
-      <c r="G164" s="6" t="s">
-        <v>671</v>
       </c>
       <c r="H164" s="6" t="s">
         <v>34</v>
@@ -8332,13 +8332,13 @@
         <v>25</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C165" s="6" t="s">
         <v>87</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E165" s="6" t="s">
         <v>76</v>
@@ -8347,7 +8347,7 @@
         <v>5135569691</v>
       </c>
       <c r="G165" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="H165" s="6" t="s">
         <v>8</v>
@@ -8374,7 +8374,7 @@
       </c>
       <c r="C166" s="6"/>
       <c r="D166" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E166" s="6" t="s">
         <v>7</v>
@@ -8383,7 +8383,7 @@
         <v>2032419629</v>
       </c>
       <c r="G166" s="6" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H166" s="6" t="s">
         <v>2</v>
@@ -8401,22 +8401,22 @@
     <row r="167" spans="1:13">
       <c r="A167" s="6"/>
       <c r="B167" s="6" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C167" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D167" s="6" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E167" s="6" t="s">
         <v>76</v>
       </c>
       <c r="F167" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="G167" s="6" t="s">
         <v>679</v>
-      </c>
-      <c r="G167" s="6" t="s">
-        <v>680</v>
       </c>
       <c r="H167" s="6" t="s">
         <v>2</v>
@@ -8438,16 +8438,16 @@
       </c>
       <c r="C168" s="6"/>
       <c r="D168" s="6" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E168" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F168" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="G168" s="6" t="s">
         <v>682</v>
-      </c>
-      <c r="G168" s="6" t="s">
-        <v>683</v>
       </c>
       <c r="H168" s="6" t="s">
         <v>34</v>
@@ -8470,20 +8470,20 @@
         <v>5</v>
       </c>
       <c r="B169" s="6" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C169" s="6"/>
       <c r="D169" s="6" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E169" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F169" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="G169" s="6" t="s">
         <v>686</v>
-      </c>
-      <c r="G169" s="6" t="s">
-        <v>687</v>
       </c>
       <c r="H169" s="6" t="s">
         <v>8</v>
@@ -8503,13 +8503,13 @@
         <v>5</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C170" s="6" t="s">
         <v>87</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E170" s="6" t="s">
         <v>30</v>
@@ -8518,7 +8518,7 @@
         <v>6308402826</v>
       </c>
       <c r="G170" s="6" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H170" s="6" t="s">
         <v>8</v>
@@ -8538,20 +8538,20 @@
         <v>25</v>
       </c>
       <c r="B171" s="6" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C171" s="6"/>
       <c r="D171" s="6" t="s">
+        <v>691</v>
+      </c>
+      <c r="E171" s="6" t="s">
         <v>692</v>
       </c>
-      <c r="E171" s="6" t="s">
+      <c r="F171" s="7" t="s">
         <v>693</v>
       </c>
-      <c r="F171" s="7" t="s">
+      <c r="G171" s="6" t="s">
         <v>694</v>
-      </c>
-      <c r="G171" s="6" t="s">
-        <v>695</v>
       </c>
       <c r="H171" s="6" t="s">
         <v>8</v>
@@ -8581,16 +8581,16 @@
       </c>
       <c r="C172" s="6"/>
       <c r="D172" s="6" t="s">
+        <v>695</v>
+      </c>
+      <c r="E172" s="6" t="s">
         <v>696</v>
       </c>
-      <c r="E172" s="6" t="s">
+      <c r="F172" s="7" t="s">
         <v>697</v>
       </c>
-      <c r="F172" s="7" t="s">
+      <c r="G172" s="6" t="s">
         <v>698</v>
-      </c>
-      <c r="G172" s="6" t="s">
-        <v>699</v>
       </c>
       <c r="H172" s="6" t="s">
         <v>24</v>
@@ -8616,13 +8616,13 @@
         <v>5</v>
       </c>
       <c r="B173" s="6" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="C173" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D173" s="6" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E173" s="6" t="s">
         <v>1</v>
@@ -8631,7 +8631,7 @@
         <v>6305064813</v>
       </c>
       <c r="G173" s="6" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="H173" s="6" t="s">
         <v>2</v>
@@ -8651,11 +8651,11 @@
         <v>25</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="C174" s="6"/>
       <c r="D174" s="6" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E174" s="6" t="s">
         <v>49</v>
@@ -8664,7 +8664,7 @@
         <v>8128333057</v>
       </c>
       <c r="G174" s="6" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="H174" s="6" t="s">
         <v>8</v>
@@ -8690,16 +8690,16 @@
         <v>15</v>
       </c>
       <c r="D175" s="6" t="s">
+        <v>705</v>
+      </c>
+      <c r="E175" s="6" t="s">
         <v>706</v>
       </c>
-      <c r="E175" s="6" t="s">
+      <c r="F175" s="7" t="s">
         <v>707</v>
       </c>
-      <c r="F175" s="7" t="s">
+      <c r="G175" s="6" t="s">
         <v>708</v>
-      </c>
-      <c r="G175" s="6" t="s">
-        <v>709</v>
       </c>
       <c r="H175" s="6" t="s">
         <v>24</v>
@@ -8722,20 +8722,20 @@
         <v>5</v>
       </c>
       <c r="B176" s="6" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C176" s="6"/>
       <c r="D176" s="6" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E176" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F176" s="7" t="s">
+        <v>711</v>
+      </c>
+      <c r="G176" s="6" t="s">
         <v>712</v>
-      </c>
-      <c r="G176" s="6" t="s">
-        <v>713</v>
       </c>
       <c r="H176" s="6" t="s">
         <v>24</v>
@@ -8755,20 +8755,20 @@
         <v>5</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C177" s="6"/>
       <c r="D177" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="E177" s="6" t="s">
         <v>715</v>
       </c>
-      <c r="E177" s="6" t="s">
+      <c r="F177" s="7" t="s">
         <v>716</v>
       </c>
-      <c r="F177" s="7" t="s">
+      <c r="G177" s="6" t="s">
         <v>717</v>
-      </c>
-      <c r="G177" s="6" t="s">
-        <v>718</v>
       </c>
       <c r="H177" s="6" t="s">
         <v>24</v>
@@ -8792,7 +8792,7 @@
       </c>
       <c r="C178" s="6"/>
       <c r="D178" s="6" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E178" s="6" t="s">
         <v>42</v>
@@ -8801,7 +8801,7 @@
         <v>9498242894</v>
       </c>
       <c r="G178" s="6" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="H178" s="6" t="s">
         <v>24</v>
@@ -8830,16 +8830,16 @@
         <v>79</v>
       </c>
       <c r="D179" s="6" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E179" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F179" s="7" t="s">
+        <v>721</v>
+      </c>
+      <c r="G179" s="6" t="s">
         <v>722</v>
-      </c>
-      <c r="G179" s="6" t="s">
-        <v>723</v>
       </c>
       <c r="H179" s="6" t="s">
         <v>8</v>
@@ -8857,20 +8857,20 @@
     <row r="180" spans="1:13">
       <c r="A180" s="6"/>
       <c r="B180" s="6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C180" s="6"/>
       <c r="D180" s="6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E180" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F180" s="7" t="s">
+        <v>725</v>
+      </c>
+      <c r="G180" s="6" t="s">
         <v>726</v>
-      </c>
-      <c r="G180" s="6" t="s">
-        <v>727</v>
       </c>
       <c r="H180" s="6" t="s">
         <v>24</v>
@@ -8890,20 +8890,20 @@
         <v>25</v>
       </c>
       <c r="B181" s="6" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C181" s="6"/>
       <c r="D181" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="E181" s="6" t="s">
         <v>729</v>
-      </c>
-      <c r="E181" s="6" t="s">
-        <v>730</v>
       </c>
       <c r="F181" s="7">
         <v>41316315146</v>
       </c>
       <c r="G181" s="6" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="H181" s="6" t="s">
         <v>8</v>
@@ -8923,20 +8923,20 @@
         <v>5</v>
       </c>
       <c r="B182" s="6" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C182" s="6"/>
       <c r="D182" s="6" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E182" s="6" t="s">
         <v>33</v>
       </c>
       <c r="F182" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="G182" s="6" t="s">
         <v>734</v>
-      </c>
-      <c r="G182" s="6" t="s">
-        <v>735</v>
       </c>
       <c r="H182" s="6" t="s">
         <v>34</v>
@@ -8960,16 +8960,16 @@
       </c>
       <c r="C183" s="6"/>
       <c r="D183" s="6" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E183" s="6" t="s">
         <v>35</v>
       </c>
       <c r="F183" s="7" t="s">
+        <v>736</v>
+      </c>
+      <c r="G183" s="6" t="s">
         <v>737</v>
-      </c>
-      <c r="G183" s="6" t="s">
-        <v>738</v>
       </c>
       <c r="H183" s="6" t="s">
         <v>2</v>
@@ -8999,10 +8999,10 @@
         <v>69</v>
       </c>
       <c r="F184" s="7" t="s">
+        <v>738</v>
+      </c>
+      <c r="G184" s="6" t="s">
         <v>739</v>
-      </c>
-      <c r="G184" s="6" t="s">
-        <v>740</v>
       </c>
       <c r="H184" s="6" t="s">
         <v>8</v>
@@ -9022,7 +9022,7 @@
         <v>5</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C185" s="6" t="s">
         <v>6</v>
@@ -9034,10 +9034,10 @@
         <v>37</v>
       </c>
       <c r="F185" s="7" t="s">
+        <v>741</v>
+      </c>
+      <c r="G185" s="6" t="s">
         <v>742</v>
-      </c>
-      <c r="G185" s="6" t="s">
-        <v>743</v>
       </c>
       <c r="H185" s="6" t="s">
         <v>2</v>
@@ -9061,16 +9061,16 @@
       </c>
       <c r="C186" s="6"/>
       <c r="D186" s="6" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E186" s="6" t="s">
         <v>81</v>
       </c>
       <c r="F186" s="7" t="s">
+        <v>744</v>
+      </c>
+      <c r="G186" s="6" t="s">
         <v>745</v>
-      </c>
-      <c r="G186" s="6" t="s">
-        <v>746</v>
       </c>
       <c r="H186" s="6" t="s">
         <v>8</v>
@@ -9093,22 +9093,22 @@
         <v>5</v>
       </c>
       <c r="B187" s="6" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C187" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D187" s="6" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E187" s="6" t="s">
         <v>49</v>
       </c>
       <c r="F187" s="7" t="s">
+        <v>748</v>
+      </c>
+      <c r="G187" s="6" t="s">
         <v>749</v>
-      </c>
-      <c r="G187" s="6" t="s">
-        <v>750</v>
       </c>
       <c r="H187" s="6" t="s">
         <v>2</v>
@@ -9134,16 +9134,16 @@
         <v>52</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E188" s="6" t="s">
         <v>70</v>
       </c>
       <c r="F188" s="7" t="s">
+        <v>751</v>
+      </c>
+      <c r="G188" s="6" t="s">
         <v>752</v>
-      </c>
-      <c r="G188" s="6" t="s">
-        <v>753</v>
       </c>
       <c r="H188" s="6" t="s">
         <v>24</v>
@@ -9175,13 +9175,13 @@
         <v>89</v>
       </c>
       <c r="E189" s="6" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F189" s="7">
         <v>9704915033</v>
       </c>
       <c r="G189" s="6" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="H189" s="6" t="s">
         <v>8</v>
@@ -9212,7 +9212,7 @@
         <v>6308402156</v>
       </c>
       <c r="G190" s="6" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="H190" s="6" t="s">
         <v>24</v>
@@ -9239,16 +9239,16 @@
       </c>
       <c r="C191" s="6"/>
       <c r="D191" s="6" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E191" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F191" s="7" t="s">
+        <v>757</v>
+      </c>
+      <c r="G191" s="6" t="s">
         <v>758</v>
-      </c>
-      <c r="G191" s="6" t="s">
-        <v>759</v>
       </c>
       <c r="H191" s="6" t="s">
         <v>2</v>
@@ -9274,16 +9274,16 @@
         <v>6</v>
       </c>
       <c r="D192" s="6" t="s">
+        <v>759</v>
+      </c>
+      <c r="E192" s="6" t="s">
         <v>760</v>
-      </c>
-      <c r="E192" s="6" t="s">
-        <v>761</v>
       </c>
       <c r="F192" s="7">
         <v>2039843993</v>
       </c>
       <c r="G192" s="6" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="H192" s="6" t="s">
         <v>8</v>
@@ -9301,11 +9301,11 @@
     <row r="193" spans="1:13">
       <c r="A193" s="6"/>
       <c r="B193" s="6" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C193" s="6"/>
       <c r="D193" s="6" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E193" s="6" t="s">
         <v>33</v>
@@ -9314,7 +9314,7 @@
         <v>6313445325</v>
       </c>
       <c r="G193" s="6" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="H193" s="6" t="s">
         <v>34</v>
@@ -9334,20 +9334,20 @@
         <v>25</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C194" s="6"/>
       <c r="D194" s="6" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E194" s="6" t="s">
         <v>83</v>
       </c>
       <c r="F194" s="7" t="s">
+        <v>767</v>
+      </c>
+      <c r="G194" s="6" t="s">
         <v>768</v>
-      </c>
-      <c r="G194" s="6" t="s">
-        <v>769</v>
       </c>
       <c r="H194" s="6" t="s">
         <v>24</v>
@@ -9367,11 +9367,11 @@
         <v>5</v>
       </c>
       <c r="B195" s="6" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C195" s="6"/>
       <c r="D195" s="6" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E195" s="6" t="s">
         <v>33</v>
@@ -9380,7 +9380,7 @@
         <v>3442870</v>
       </c>
       <c r="G195" s="6" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H195" s="6" t="s">
         <v>34</v>
@@ -9400,13 +9400,13 @@
         <v>19</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C196" s="6" t="s">
         <v>72</v>
       </c>
       <c r="D196" s="6" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E196" s="6" t="s">
         <v>11</v>
@@ -9415,7 +9415,7 @@
         <v>5402315634</v>
       </c>
       <c r="G196" s="6" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H196" s="6" t="s">
         <v>2</v>
@@ -9435,20 +9435,20 @@
         <v>5</v>
       </c>
       <c r="B197" s="6" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C197" s="6"/>
       <c r="D197" s="6" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E197" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F197" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="G197" s="6" t="s">
         <v>778</v>
-      </c>
-      <c r="G197" s="6" t="s">
-        <v>779</v>
       </c>
       <c r="H197" s="6" t="s">
         <v>24</v>
@@ -9475,16 +9475,16 @@
       </c>
       <c r="C198" s="6"/>
       <c r="D198" s="6" t="s">
+        <v>779</v>
+      </c>
+      <c r="E198" s="6" t="s">
         <v>780</v>
       </c>
-      <c r="E198" s="6" t="s">
+      <c r="F198" s="7" t="s">
         <v>781</v>
       </c>
-      <c r="F198" s="7" t="s">
+      <c r="G198" s="6" t="s">
         <v>782</v>
-      </c>
-      <c r="G198" s="6" t="s">
-        <v>783</v>
       </c>
       <c r="H198" s="6" t="s">
         <v>8</v>
@@ -9502,7 +9502,7 @@
     <row r="199" spans="1:13">
       <c r="A199" s="6"/>
       <c r="B199" s="6" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C199" s="6"/>
       <c r="D199" s="6" t="s">
@@ -9512,10 +9512,10 @@
         <v>33</v>
       </c>
       <c r="F199" s="7" t="s">
+        <v>784</v>
+      </c>
+      <c r="G199" s="6" t="s">
         <v>785</v>
-      </c>
-      <c r="G199" s="6" t="s">
-        <v>786</v>
       </c>
       <c r="H199" s="6" t="s">
         <v>34</v>
@@ -9538,7 +9538,7 @@
         <v>25</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C200" s="6"/>
       <c r="D200" s="6" t="s">
@@ -9548,10 +9548,10 @@
         <v>41</v>
       </c>
       <c r="F200" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="G200" s="6" t="s">
         <v>788</v>
-      </c>
-      <c r="G200" s="6" t="s">
-        <v>789</v>
       </c>
       <c r="H200" s="6" t="s">
         <v>8</v>
@@ -9571,11 +9571,11 @@
         <v>5</v>
       </c>
       <c r="B201" s="6" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C201" s="6"/>
       <c r="D201" s="6" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E201" s="6" t="s">
         <v>33</v>
@@ -9584,7 +9584,7 @@
         <v>6313448320</v>
       </c>
       <c r="G201" s="6" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="H201" s="6" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
add middle initial to Raaf
</commit_message>
<xml_diff>
--- a/other/reginfo.xlsx
+++ b/other/reginfo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="771">
   <si>
     <t>Mr.</t>
   </si>
@@ -2712,8 +2712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M195"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77:XFD77"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C139" sqref="C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -6187,7 +6187,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="409.6">
+    <row r="103" spans="1:13">
       <c r="A103" s="6" t="s">
         <v>19</v>
       </c>
@@ -7392,7 +7392,9 @@
       <c r="B139" s="6" t="s">
         <v>580</v>
       </c>
-      <c r="C139" s="6"/>
+      <c r="C139" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="D139" s="6" t="s">
         <v>581</v>
       </c>

</xml_diff>